<commit_message>
Simplify the prove assignments for the student chosen program in lessons 11 - 13.
</commit_message>
<xml_diff>
--- a/docs/prove_rubrics.xlsx
+++ b/docs/prove_rubrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rab29\cse111\cse111-course\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947BC7A2-9C45-453A-9B4A-D88CDD8DCC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60651964-8DEB-41B2-A4C6-CECC54CD96BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12360" yWindow="1005" windowWidth="16380" windowHeight="10785" xr2:uid="{83A43617-33C9-497C-BBF7-28C4448D3B5F}"/>
+    <workbookView xWindow="11445" yWindow="1860" windowWidth="17295" windowHeight="12390" firstSheet="8" activeTab="10" xr2:uid="{83A43617-33C9-497C-BBF7-28C4448D3B5F}"/>
   </bookViews>
   <sheets>
     <sheet name="milestone01" sheetId="5" r:id="rId1"/>
@@ -21,6 +21,12 @@
     <sheet name="prove06" sheetId="9" r:id="rId6"/>
     <sheet name="milestone07" sheetId="7" r:id="rId7"/>
     <sheet name="prove08" sheetId="4" r:id="rId8"/>
+    <sheet name="milestone09" sheetId="10" r:id="rId9"/>
+    <sheet name="prove10" sheetId="11" r:id="rId10"/>
+    <sheet name="milestone11" sheetId="12" r:id="rId11"/>
+    <sheet name="milestone12" sheetId="13" r:id="rId12"/>
+    <sheet name="prove13" sheetId="14" r:id="rId13"/>
+    <sheet name="prove14" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="308">
   <si>
     <t>Complete (100%)</t>
   </si>
@@ -533,6 +539,438 @@
   </si>
   <si>
     <t>Program prints the total number of protons in a molecule of the user given formula</t>
+  </si>
+  <si>
+    <t>Program includes some other functionality</t>
+  </si>
+  <si>
+    <t>Program contains a function named read_dict that reads the contents of a CSV file into a new compound dictionary and returns the dictionary</t>
+  </si>
+  <si>
+    <t>The read_dict function exists but doesn't completely or correctly read the CSV file into a compound dictionary or the function doesn't return the dictionary</t>
+  </si>
+  <si>
+    <t>The read_dict function returns a compound dictionary as described in the assignment. Both students and graders can verify this with the test program that is given in the assignment</t>
+  </si>
+  <si>
+    <t>No attempt to write the read_dict function</t>
+  </si>
+  <si>
+    <t>The main function calls the read_dict function and prints the returned products dictionary</t>
+  </si>
+  <si>
+    <t>Program contains a function named main that calls the read_dict function and then prints the returned products dictionary</t>
+  </si>
+  <si>
+    <t>No attempt to call the read_dict function</t>
+  </si>
+  <si>
+    <t>The main function exists but doesn't call the read_dict function or it doesn't print the returned products dictionary</t>
+  </si>
+  <si>
+    <t>No attempt to open the requests.csv file</t>
+  </si>
+  <si>
+    <t>The main function includes an incorrect attempt to open the requests.csv file</t>
+  </si>
+  <si>
+    <t>The main function opens the requests.csv file for reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The main function contains a loop that reads from the requests.csv file </t>
+  </si>
+  <si>
+    <t>Within the loop, the program uses a requested product number to find the corresponding item in the products dictionary</t>
+  </si>
+  <si>
+    <t>Within the loop, the program prints the product name, requested quantity, and product price</t>
+  </si>
+  <si>
+    <t>The main function includes a call to the open function and correctly opens the requests.csv file for reading</t>
+  </si>
+  <si>
+    <t>The main function includes an incorrect loop to read from the requests.csv file</t>
+  </si>
+  <si>
+    <t>No attempt to read from the requests.csv file</t>
+  </si>
+  <si>
+    <t>No attempt to find an item in the products dictionary</t>
+  </si>
+  <si>
+    <t>The program uses a requested product number to find the corresponding item in the products dictionary</t>
+  </si>
+  <si>
+    <t>The program prints the product name, requested quantity, and product price</t>
+  </si>
+  <si>
+    <t>No attempt to print the product name, requested quantity, or product price</t>
+  </si>
+  <si>
+    <t>The main function includes an incorrect attempt to find an item in the dictionary</t>
+  </si>
+  <si>
+    <t>The main function prints at least one of the product name, requested quantity, or product price</t>
+  </si>
+  <si>
+    <t>Program prints a store name at the top of the receipt</t>
+  </si>
+  <si>
+    <t>No attempt made to print a store name</t>
+  </si>
+  <si>
+    <t>Program prints a store name</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>Program prints a list of products requested by the customer</t>
+  </si>
+  <si>
+    <t>Program prints a list of products requested by the customer as shown in the sample output for this assignment</t>
+  </si>
+  <si>
+    <t>No attempt made to print the list of sample products</t>
+  </si>
+  <si>
+    <t>Program prints an incomplete or incorrect list of products</t>
+  </si>
+  <si>
+    <t>Program computes and prints the number of items</t>
+  </si>
+  <si>
+    <t>No attempt made to compute or print the number of items</t>
+  </si>
+  <si>
+    <t>Program computes and prints the correct number of items</t>
+  </si>
+  <si>
+    <t>Program computes and prints an incorrect number of items</t>
+  </si>
+  <si>
+    <t>Program computes and prints the subtotal</t>
+  </si>
+  <si>
+    <t>Program computes and prints the correct subtotal</t>
+  </si>
+  <si>
+    <t>Program computes and prints an incorrect subtotal</t>
+  </si>
+  <si>
+    <t>No attempt made to compute or print the subtotal</t>
+  </si>
+  <si>
+    <t>Program computes and prints the sales tax</t>
+  </si>
+  <si>
+    <t>Program computes and prints the correct sales tax</t>
+  </si>
+  <si>
+    <t>Program computes and prints an incorrect sales tax</t>
+  </si>
+  <si>
+    <t>No attempt made to compute or print the sales tax</t>
+  </si>
+  <si>
+    <t>Program computes and prints the total</t>
+  </si>
+  <si>
+    <t>Program computes and prints the correct total</t>
+  </si>
+  <si>
+    <t>Program computes and prints an incorrect total</t>
+  </si>
+  <si>
+    <t>No attempt made to compute or print the total</t>
+  </si>
+  <si>
+    <t>No attempt made to print a thank you message</t>
+  </si>
+  <si>
+    <t>Program prints a thank you message</t>
+  </si>
+  <si>
+    <t>Program prints a thank you message near the bottom of the receipt</t>
+  </si>
+  <si>
+    <t>Program prints the current date and time</t>
+  </si>
+  <si>
+    <t>Program prints the current date and time in the format specified in the assignment</t>
+  </si>
+  <si>
+    <t>Program prints the wrong date or the current date in a format different from the one specified in the assignment</t>
+  </si>
+  <si>
+    <t>No attempt made to print the current date and time</t>
+  </si>
+  <si>
+    <t>Program contains a try block</t>
+  </si>
+  <si>
+    <t>Program doesn't include any try block</t>
+  </si>
+  <si>
+    <t>Program contains an except block to handle KeyError</t>
+  </si>
+  <si>
+    <t>Program contains an except block to handle FileNotFoundError</t>
+  </si>
+  <si>
+    <t>Program contains an except block to handle KeyError that prints an error message very similar to the one shown in this assignment</t>
+  </si>
+  <si>
+    <t>Program contains an except block to handle FileNotFoundError that prints an error message very similar to the one shown in this assignment</t>
+  </si>
+  <si>
+    <t>Program contains at least one try block but not all statements that might raise a FileNotFoundError or a KeyError are contained within a try block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program contains at least one try block and all statements that might raise a FileNotFoundError or a KeyError are contained within a try block or within a user-defined function that is called within a try block </t>
+  </si>
+  <si>
+    <t>Program contains an except block to handle KeyError, but the block doesn't print a message like the one shown in this assignment</t>
+  </si>
+  <si>
+    <t>Program doesn't include an except block to handle KeyError</t>
+  </si>
+  <si>
+    <t>Program contains an except block to handle FileNotFoundError, but the block doesn't print a message like the one shown in this assignment</t>
+  </si>
+  <si>
+    <t>Program doesn't include an except block to handle FileNotFoundError</t>
+  </si>
+  <si>
+    <t>Title of student chosen program</t>
+  </si>
+  <si>
+    <t>Real world problem</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Python modules</t>
+  </si>
+  <si>
+    <t>Program functions</t>
+  </si>
+  <si>
+    <t>Test functions</t>
+  </si>
+  <si>
+    <t>Table of Work</t>
+  </si>
+  <si>
+    <t>The table of work is organized and makes sense</t>
+  </si>
+  <si>
+    <t>Developing (75%)</t>
+  </si>
+  <si>
+    <t>Developing (25%)</t>
+  </si>
+  <si>
+    <t>Program function names</t>
+  </si>
+  <si>
+    <t>Test function names</t>
+  </si>
+  <si>
+    <t>Best practices for functions</t>
+  </si>
+  <si>
+    <t>No title or a title like "I don't know"</t>
+  </si>
+  <si>
+    <t>No real world problem listed or something like "I don't know"</t>
+  </si>
+  <si>
+    <t>No answer</t>
+  </si>
+  <si>
+    <t>No answer or something like "My program doesn't need multiple functions"</t>
+  </si>
+  <si>
+    <t>No answer or something like "My program doesn't need test functions"</t>
+  </si>
+  <si>
+    <t>Answer contains the name of at least one Python module</t>
+  </si>
+  <si>
+    <t>Answer contains at least one sentence or a list describing what the student intends to learn</t>
+  </si>
+  <si>
+    <t>Answer contains a real world problem that the student's program will address.</t>
+  </si>
+  <si>
+    <t>Answer contains a title</t>
+  </si>
+  <si>
+    <t>Answer is "yes" or something very close to "yes"</t>
+  </si>
+  <si>
+    <t>Student reported time in the table of work totals to at least 4 hours</t>
+  </si>
+  <si>
+    <t>Reported time totals to at least 3 hours</t>
+  </si>
+  <si>
+    <t>Reported time totals to at least 2 hours</t>
+  </si>
+  <si>
+    <t>The report contains a table of work, but it has very few details or doesn't make sense</t>
+  </si>
+  <si>
+    <t>No table of work</t>
+  </si>
+  <si>
+    <t>Reported time totals to at least 1 hour</t>
+  </si>
+  <si>
+    <t>Answer contains three or more function names</t>
+  </si>
+  <si>
+    <t>Answer contains two or one fuction names</t>
+  </si>
+  <si>
+    <t>All of the best practice questions are answered with "yes" or the answer contains the student's plan to change her program's functions</t>
+  </si>
+  <si>
+    <t>One or more of the best practice questions are not answered or not answered with "yes" and the answer doesn't contain a plan to change the program's functions</t>
+  </si>
+  <si>
+    <t>Answer contains one or more test function names</t>
+  </si>
+  <si>
+    <t>Answer is something like "I'm not sure how to write test functions"</t>
+  </si>
+  <si>
+    <t>No reported time or the reported work time totals to less than 1 hour</t>
+  </si>
+  <si>
+    <t>Answer is something like "I don't know" or "I'm not sure"</t>
+  </si>
+  <si>
+    <t>Answer is something like "maybe", "I'll try", or "if I have time"</t>
+  </si>
+  <si>
+    <t>Student reported time in the table of work totals to at least 6 hours</t>
+  </si>
+  <si>
+    <t>Reported time totals to at least 5 hours</t>
+  </si>
+  <si>
+    <t>Developing (83%)</t>
+  </si>
+  <si>
+    <t>Developing (67%)</t>
+  </si>
+  <si>
+    <t>Reported time totals to at least 4 hours</t>
+  </si>
+  <si>
+    <t>Developing (17%)</t>
+  </si>
+  <si>
+    <t>Developing (33%)</t>
+  </si>
+  <si>
+    <t>Work times in table of work</t>
+  </si>
+  <si>
+    <t>Program is divided into functions</t>
+  </si>
+  <si>
+    <t>Program effectively uses existing Python modules</t>
+  </si>
+  <si>
+    <t>Program uses 1 or more existing Python modules such as math, random, csv, requests, pandas, and tkinter</t>
+  </si>
+  <si>
+    <t>Program Python file wasn't submitted</t>
+  </si>
+  <si>
+    <t>Test function coverage</t>
+  </si>
+  <si>
+    <t>Python test file contains 2 or more test functions that each test one program function</t>
+  </si>
+  <si>
+    <t>Program runs, produces correct results</t>
+  </si>
+  <si>
+    <t>Program doesn't run or produces incorrect results</t>
+  </si>
+  <si>
+    <t>Program Python file wasn't submitted or counting the main function, the program has only 0 or 1 functions</t>
+  </si>
+  <si>
+    <t>Program Python file wasn't submitted or the program doesn't use any existing Python modules</t>
+  </si>
+  <si>
+    <t>No test file or the test file contains no test functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each test function contains at least 2 calls and 2 asserts </t>
+  </si>
+  <si>
+    <t>Test functions pass</t>
+  </si>
+  <si>
+    <t>Number of test functions</t>
+  </si>
+  <si>
+    <t>All test functions pass</t>
+  </si>
+  <si>
+    <t>One or more test functions don't pass</t>
+  </si>
+  <si>
+    <t>No test file or none of the test functions pass</t>
+  </si>
+  <si>
+    <t>Test file contains only 1 test function</t>
+  </si>
+  <si>
+    <t>Counting the main function, the program is divided into 4 or more functions</t>
+  </si>
+  <si>
+    <t>Counting the main function, the program is divided into 3 or fewer functions</t>
+  </si>
+  <si>
+    <t>One or more test functions contain only 1 call and 1 assert</t>
+  </si>
+  <si>
+    <t>No test file or at least one of the test functions is empty (contains no assert statement)</t>
+  </si>
+  <si>
+    <t>Program runs correctly</t>
+  </si>
+  <si>
+    <t>Power of functions</t>
+  </si>
+  <si>
+    <t>Answer contains two or more sentences describing the student's experience with functions</t>
+  </si>
+  <si>
+    <t>Answer contains only one sentence</t>
+  </si>
+  <si>
+    <t>Value of test functions</t>
+  </si>
+  <si>
+    <t>Answer contains two or more sentences explaining the value of test functions</t>
+  </si>
+  <si>
+    <t>Troubleshooting</t>
+  </si>
+  <si>
+    <t>Answer contains two or more sentences explaining how the student troubleshoots a program that isn't working</t>
+  </si>
+  <si>
+    <t>No answer or answer is something like "I didn't have time" or "my program doesn't need test functions"</t>
   </si>
 </sst>
 </file>
@@ -909,17 +1347,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3F81A9-7669-4070-9361-3FCA18DE0127}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="6" width="6.77734375" customWidth="1"/>
+    <col min="1" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -939,7 +1378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -960,7 +1399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -981,7 +1420,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1002,7 +1441,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1026,6 +1465,1066 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A098B1-E65D-4528-8482-60DFE9F53BCF}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="4">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4">
+        <f>E2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="4">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F12" si="0">F2 + E3</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" s="4">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5" s="4">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6" s="4">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E7" s="4">
+        <v>8</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E9" s="4">
+        <v>8</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E10" s="4">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="4">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12" s="4">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C737A82-9DDF-4917-9FC5-3513F4A9CF88}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E2" s="4">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4">
+        <f>E2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F7" si="0">F2 + E3</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD271EA-8134-4F80-B747-0537BC177E6B}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="7" max="8" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G2" s="4">
+        <v>2</v>
+      </c>
+      <c r="H2" s="4">
+        <f>G2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="G3" s="4">
+        <v>10</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H6" si="0">H2 + G3</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C73B502-4F5A-46F6-9EBA-FFA9EF6B5ED8}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" customWidth="1"/>
+    <col min="9" max="10" width="7.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="I2" s="4">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4">
+        <f>I2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="I3" s="4">
+        <v>50</v>
+      </c>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J9" si="0">J2 + I3</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="I4" s="4">
+        <v>10</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="I5" s="4">
+        <v>10</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="I6" s="4">
+        <v>5</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="I7" s="4">
+        <v>5</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="I8" s="4">
+        <v>5</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="I9" s="4">
+        <v>5</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8697553C-A0C9-4EA9-BCCB-F99FEBFB2CE0}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4">
+        <f>E2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E3" s="4">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3" si="0">F2 + E3</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E4" s="4">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" ref="F4" si="1">F3 + E4</f>
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1034,16 +2533,17 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="6" width="6.77734375" customWidth="1"/>
+    <col min="1" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1063,7 +2563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1084,7 +2584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1105,7 +2605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1126,7 +2626,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1147,7 +2647,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>76</v>
       </c>
@@ -1168,7 +2668,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>155</v>
       </c>
@@ -1189,7 +2689,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>156</v>
       </c>
@@ -1210,7 +2710,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1231,7 +2731,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -1252,21 +2752,21 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14" s="3"/>
     </row>
   </sheetData>
@@ -1280,16 +2780,17 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="6" width="6.77734375" customWidth="1"/>
+    <col min="1" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1309,7 +2810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
@@ -1330,7 +2831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -1351,7 +2852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
@@ -1372,7 +2873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>83</v>
       </c>
@@ -1403,17 +2904,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB49666-F403-4087-9EDE-CA904292F4FF}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="6" width="6.77734375" customWidth="1"/>
+    <col min="1" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1433,7 +2935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
@@ -1454,7 +2956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -1475,7 +2977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
@@ -1496,7 +2998,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>83</v>
       </c>
@@ -1517,7 +3019,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
@@ -1538,7 +3040,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -1559,7 +3061,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>43</v>
       </c>
@@ -1580,7 +3082,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -1601,7 +3103,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
@@ -1622,7 +3124,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>47</v>
       </c>
@@ -1643,10 +3145,10 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
@@ -1656,7 +3158,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
@@ -1671,7 +3173,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1686,7 +3188,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1702,17 +3204,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6133947E-7855-47EB-8E32-C4C69749B32C}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="6" width="6.77734375" customWidth="1"/>
+    <col min="1" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1732,7 +3235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>122</v>
       </c>
@@ -1753,7 +3256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>110</v>
       </c>
@@ -1774,7 +3277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>114</v>
       </c>
@@ -1795,7 +3298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>115</v>
       </c>
@@ -1816,7 +3319,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>125</v>
       </c>
@@ -1837,7 +3340,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>126</v>
       </c>
@@ -1858,7 +3361,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>127</v>
       </c>
@@ -1889,17 +3392,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB93CC9-808E-49AC-9CFB-DAB4817F9750}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="6" width="6.77734375" customWidth="1"/>
+    <col min="1" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1919,7 +3423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>153</v>
       </c>
@@ -1940,7 +3444,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>110</v>
       </c>
@@ -1961,7 +3465,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>114</v>
       </c>
@@ -1982,7 +3486,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>115</v>
       </c>
@@ -2003,7 +3507,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>149</v>
       </c>
@@ -2024,7 +3528,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>148</v>
       </c>
@@ -2045,7 +3549,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>125</v>
       </c>
@@ -2066,7 +3570,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>126</v>
       </c>
@@ -2087,7 +3591,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>127</v>
       </c>
@@ -2108,7 +3612,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>137</v>
       </c>
@@ -2129,7 +3633,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>141</v>
       </c>
@@ -2150,27 +3654,27 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>160</v>
       </c>
@@ -2186,16 +3690,17 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="6" width="6.77734375" customWidth="1"/>
+    <col min="1" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2215,7 +3720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>98</v>
       </c>
@@ -2236,7 +3741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>161</v>
       </c>
@@ -2268,16 +3773,17 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="6" width="6.77734375" customWidth="1"/>
+    <col min="1" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2297,7 +3803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
@@ -2318,7 +3824,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>55</v>
       </c>
@@ -2335,11 +3841,11 @@
         <v>10</v>
       </c>
       <c r="F3" s="4">
-        <f>F2 + E3</f>
+        <f t="shared" ref="F3:F8" si="0">F2 + E3</f>
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>54</v>
       </c>
@@ -2356,11 +3862,11 @@
         <v>10</v>
       </c>
       <c r="F4" s="4">
-        <f>F3 + E4</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>60</v>
       </c>
@@ -2377,11 +3883,11 @@
         <v>20</v>
       </c>
       <c r="F5" s="4">
-        <f>F4 + E5</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>108</v>
       </c>
@@ -2398,11 +3904,11 @@
         <v>13</v>
       </c>
       <c r="F6" s="4">
-        <f>F5 + E6</f>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>106</v>
       </c>
@@ -2419,11 +3925,11 @@
         <v>10</v>
       </c>
       <c r="F7" s="4">
-        <f>F6 + E7</f>
+        <f t="shared" si="0"/>
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>107</v>
       </c>
@@ -2440,28 +3946,195 @@
         <v>20</v>
       </c>
       <c r="F8" s="4">
-        <f>F7 + E8</f>
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE4A075-B6A7-44BB-ABC7-43EDB8FD44F8}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="4">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4">
+        <f>E2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4">
+        <f>F2 + E3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" ref="F4:F7" si="0">F3 + E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="4">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>